<commit_message>
Fixed cumulative xs for 58Co. This resolved some issues with the beam currents, but it is something wrong as the variance minimization cant find a good dp value
</commit_message>
<xml_diff>
--- a/fit_peak_files/Peak_analysis_comments.xlsx
+++ b/fit_peak_files/Peak_analysis_comments.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/fit_peak_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="543" documentId="8_{D38E236D-DAD2-7446-A416-14A1BAF7A09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85841EC6-39D4-FB4C-A0B4-CF5077517D69}"/>
+  <xr:revisionPtr revIDLastSave="611" documentId="8_{D38E236D-DAD2-7446-A416-14A1BAF7A09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F896D3AC-4667-2A41-BDE6-C0AB192CFFC3}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{D2162805-4197-3249-B537-CF0AE71186C3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D2162805-4197-3249-B537-CF0AE71186C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="30 MeV" sheetId="1" r:id="rId1"/>
+    <sheet name="50 MeV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
   <si>
     <t>Comment</t>
   </si>
@@ -467,9 +468,6 @@
     </r>
   </si>
   <si>
-    <t>don't know, small, not small for BI_Zr05</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">BR_Zr02, </t>
     </r>
@@ -790,9 +788,6 @@
     </r>
   </si>
   <si>
-    <t>don't know, small, not small for BI_Zr05 and CR_Zr04</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">CH_Zr03, </t>
     </r>
@@ -1008,6 +1003,48 @@
   </si>
   <si>
     <t>Live time</t>
+  </si>
+  <si>
+    <t>don't know, small, might be 91NBm</t>
+  </si>
+  <si>
+    <t>don't know, small, might be 95Zr</t>
+  </si>
+  <si>
+    <t>don't know, might be 95Nb</t>
+  </si>
+  <si>
+    <t>don't know, small, might be 95NBm</t>
+  </si>
+  <si>
+    <t>don't know, small, not small for BI_Zr04, kanskje 89Nb, men gir ikke mening at den er størst i BI</t>
+  </si>
+  <si>
+    <t>don't know, small, not small for BI_Zr05 and CR_Zr04, might be 95Zr, 90Nb or 89Nb, men burde være langlivet så 95Zr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 96Nb</t>
+  </si>
+  <si>
+    <t>96Nb</t>
+  </si>
+  <si>
+    <t>small, not small for BI_Zr04, might be 96Nb, burde vært mindre intens enn 778</t>
+  </si>
+  <si>
+    <t>small, 96Nb</t>
+  </si>
+  <si>
+    <t>small, not small for BI_Zr05 might be 96Nb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small, not small for BI_Zr05, 96Nb </t>
+  </si>
+  <si>
+    <t>88Y</t>
+  </si>
+  <si>
+    <t>don't know, 27Mg from Al frames</t>
   </si>
 </sst>
 </file>
@@ -1312,13 +1349,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1335,9 +1370,7 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1356,8 +1389,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1368,12 +1401,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1403,6 +1439,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1702,17 +1742,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EAB0204-B451-8F42-930D-BA7D94248E53}">
-  <dimension ref="A3:I65"/>
+  <dimension ref="A3:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="3" max="3" width="98" customWidth="1"/>
     <col min="4" max="4" width="51.1640625" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
@@ -1865,7 +1905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1876,7 +1916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1887,8 +1927,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1898,21 +1938,20 @@
       <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" s="58"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F20" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1920,45 +1959,45 @@
         <v>236</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="26">
+      <c r="G21" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="22">
         <v>477</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="14">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="12">
         <v>241</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="15" t="s">
+      <c r="C22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="28">
+      <c r="G22" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="24">
         <v>1881</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1968,43 +2007,43 @@
       <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="30">
+      <c r="G23" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="26">
         <v>146580</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="10">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="8">
         <v>353</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="32">
+      <c r="G24" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="28">
         <v>7499</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2014,278 +2053,278 @@
       <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="51" t="s">
+      <c r="G25" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="30">
+        <v>6432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="8">
+        <v>372</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="32">
+        <v>137373</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="8">
+        <v>460</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="H25" s="34">
-        <v>6432</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="18">
-        <v>372</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="52" t="s">
+      <c r="H27" s="34">
+        <v>8898</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="8">
+        <v>481</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="36">
+        <v>225399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="8">
+        <v>569</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="36">
-        <v>137373</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27">
-        <v>460</v>
-      </c>
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="53" t="s">
+      <c r="H29" s="38">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="8">
+        <v>652</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="38">
-        <v>8898</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28">
-        <v>481</v>
-      </c>
-      <c r="C28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="57" t="s">
+      <c r="H30" s="40">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="16">
+        <v>658</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="40">
-        <v>225399</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="18">
-        <v>569</v>
-      </c>
-      <c r="C29" s="18" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="8">
+        <v>720</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="57" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="54">
+        <v>724</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="16">
+        <v>744</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="42">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="10">
-        <v>652</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="H30" s="44">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="18">
-        <v>658</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="G31" s="60" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32">
-        <v>720</v>
-      </c>
-      <c r="C32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33">
-        <v>724</v>
-      </c>
-      <c r="C33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="4" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="54">
+        <v>757</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="16">
+        <v>766</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="18">
-        <v>744</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="18">
-        <v>757</v>
-      </c>
-      <c r="C35" s="18" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="8">
+        <v>778</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="8">
+        <v>810</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="57" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="8">
+        <v>850</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="58" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="8">
+        <v>898</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="58" t="s">
         <v>48</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" s="18">
-        <v>766</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37">
-        <v>778</v>
-      </c>
-      <c r="C37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="18">
-        <v>810</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="18">
-        <v>850</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" s="18">
-        <v>898</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2303,87 +2342,87 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="18">
+      <c r="A42" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="16">
         <v>951</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" s="18">
+      <c r="A43" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="8">
         <v>1015</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="8">
+        <v>1092</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="16">
+        <v>1149</v>
+      </c>
+      <c r="C45" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" s="18">
-        <v>1092</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" s="24" t="s">
+      <c r="D45" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="8">
+        <v>1164</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="8">
+        <v>1200</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" s="55" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="18">
-        <v>1149</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" s="10">
-        <v>1164</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47">
-        <v>1200</v>
-      </c>
-      <c r="C47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2394,9 +2433,9 @@
         <v>1205</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2410,35 +2449,35 @@
       <c r="C49" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="18">
+      <c r="A50" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="16">
         <v>1275</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="10">
+      <c r="A51" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="8">
         <v>1296</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2452,22 +2491,22 @@
       <c r="C52" t="s">
         <v>23</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53" s="10">
+      <c r="A53" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="8">
         <v>1369</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="12" t="s">
+      <c r="C53" s="8" t="s">
         <v>53</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2480,21 +2519,21 @@
       <c r="C54" t="s">
         <v>23</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55">
+      <c r="A55" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="8">
         <v>1498</v>
       </c>
-      <c r="C55" t="s">
-        <v>23</v>
-      </c>
-      <c r="D55" s="6" t="s">
+      <c r="C55" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="56" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2527,31 +2566,31 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="10">
+      <c r="A58" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" s="8">
         <v>1675</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D58" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" s="18">
+      <c r="A59" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="16">
         <v>1730</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="23" t="s">
-        <v>52</v>
+      <c r="D59" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2564,21 +2603,21 @@
       <c r="C60" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="10">
+      <c r="A61" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="8">
         <v>1807</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2592,54 +2631,66 @@
       <c r="C62" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="12">
+        <v>2612</v>
+      </c>
+      <c r="C63" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B63" s="14">
-        <v>2612</v>
-      </c>
-      <c r="C63" s="14" t="s">
+      <c r="D63" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="12">
+        <v>2616</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="8">
+        <v>2751</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="14">
-        <v>2616</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B65" s="10">
-        <v>2751</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>52</v>
+      <c r="D65" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17CA361-77E0-B94C-8889-2F572D42E4DC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I started on the 50MeV analysis
</commit_message>
<xml_diff>
--- a/fit_peak_files/Peak_analysis_comments.xlsx
+++ b/fit_peak_files/Peak_analysis_comments.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/fit_peak_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="611" documentId="8_{D38E236D-DAD2-7446-A416-14A1BAF7A09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F896D3AC-4667-2A41-BDE6-C0AB192CFFC3}"/>
+  <xr:revisionPtr revIDLastSave="995" documentId="8_{D38E236D-DAD2-7446-A416-14A1BAF7A09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2439935D-4447-024E-83B9-64B81A4E41BC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D2162805-4197-3249-B537-CF0AE71186C3}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{D2162805-4197-3249-B537-CF0AE71186C3}"/>
   </bookViews>
   <sheets>
     <sheet name="30 MeV" sheetId="1" r:id="rId1"/>
     <sheet name="50 MeV" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="143">
   <si>
     <t>Comment</t>
   </si>
@@ -1045,13 +1045,844 @@
   </si>
   <si>
     <t>don't know, 27Mg from Al frames</t>
+  </si>
+  <si>
+    <t>AJ_Zr06</t>
+  </si>
+  <si>
+    <t>AL_Zr06</t>
+  </si>
+  <si>
+    <t>BQ_Zr06</t>
+  </si>
+  <si>
+    <t>CA_Zr06</t>
+  </si>
+  <si>
+    <t>AI_Zr07</t>
+  </si>
+  <si>
+    <t>AO_Zr07</t>
+  </si>
+  <si>
+    <t>AS_Zr07</t>
+  </si>
+  <si>
+    <t>CB_Zr07</t>
+  </si>
+  <si>
+    <t>AH_Zr08</t>
+  </si>
+  <si>
+    <t>AU_Zr08</t>
+  </si>
+  <si>
+    <t>CD_Zr08</t>
+  </si>
+  <si>
+    <t>AG_Zr09</t>
+  </si>
+  <si>
+    <t>AV_Zr09</t>
+  </si>
+  <si>
+    <t>CN_Zr09</t>
+  </si>
+  <si>
+    <t>AF_Zr10</t>
+  </si>
+  <si>
+    <t>AW_Zr10</t>
+  </si>
+  <si>
+    <t>CV02_Zr10</t>
+  </si>
+  <si>
+    <t>CV08_Zr10</t>
+  </si>
+  <si>
+    <t>02/13/2017 08:05:57</t>
+  </si>
+  <si>
+    <t>02/15/2017 11:16:48</t>
+  </si>
+  <si>
+    <t>02/19/2017 16:34:24</t>
+  </si>
+  <si>
+    <t>02/13/2017 08:51:14</t>
+  </si>
+  <si>
+    <t>02/13/2017 12:27:15</t>
+  </si>
+  <si>
+    <t>02/21/2017 09:51:10</t>
+  </si>
+  <si>
+    <t>02/13/2017 12:44:06</t>
+  </si>
+  <si>
+    <t>02/22/2017 17:47:49</t>
+  </si>
+  <si>
+    <t>02/13/2017 13:01:27</t>
+  </si>
+  <si>
+    <t>02/13/2017 13:37:52</t>
+  </si>
+  <si>
+    <r>
+      <t>03/07/2017  15:44:52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>03/06/2017  19:50:56</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>02/12/2017  20:51:39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>03/01/2017  17:41:55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>02/12/2017  21:05:31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>02/12/2017  21:26:24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>02/12/2017  21:39:09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>02/12/2017  21:54:20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>02/12/2017 19:21:00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>most intensive peak of 86Y, but it is more than 10 half lives after EOB</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CA_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF34BE"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CB_Zr07</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CA_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFDD270F"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AI_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF34BE"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">CB_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CD_Zr08</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BQ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AS_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AU_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF9F88"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AV_Zr09 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CB_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CN_Zr09</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AJ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFDD270F"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AI_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD861F2"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AH_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AG_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF30EA81"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AF_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AJ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFDD270F"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AI_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD861F2"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AH_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AG_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF9F88"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AV_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF30EA81"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AF_Zr10, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3138DA"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AW_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <t>AW_Zr10 and more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AW_Zr10 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AL_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF8B00"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">BQ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AO_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AS_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AU_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF9F88"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AV_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3138DA"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AW_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AJ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AL_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF8B00"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>BQ_Zr06,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFDD270F"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AI_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AO_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AS_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD861F2"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AH_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AU_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AG_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF9F88"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AV_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF30EA81"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AF_Zr10, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3138DA"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AW_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BQ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AO_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AS_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AU_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF9F88"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AV_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF30EA81"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AF_Zr10, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3138DA"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AW_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AJ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF8B00"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">BQ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFDD270F"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AI_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AO_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AS_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD861F2"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AH_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AU_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AG_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF9F88"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AV_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF30EA81"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AF_Zr10, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3138DA"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AW_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AL_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF8B00"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">BQ_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AO_Zr07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AS_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AU_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF9F88"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">AV_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3138DA"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AW_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <t>small, not small for CV02</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CN_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CV02_Zr10,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA45CD8"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD86295"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CV08_Zr10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CA_Zr06, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF34BE"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">CB_Zr07, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">CD_Zr08, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">CN_Zr09, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">CV02_Zr10, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD86295"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CV08_Zr10</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1185,6 +2016,172 @@
       <sz val="12"/>
       <color rgb="FFD861F2"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="0.79998168889431442"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF8B00"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF8B00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDD270F"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDD270F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF34BE"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF34BE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF9F88"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF9F88"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF30EA81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF30EA81"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3138DA"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3138DA"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA45CD8"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD86295"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD86295"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1349,10 +2346,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1410,6 +2408,75 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="25" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="27" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="32" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="43" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="45" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="49" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,16 +2485,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF8681"/>
-      <color rgb="FF098C40"/>
-      <color rgb="FFD861F2"/>
-      <color rgb="FFFF009D"/>
-      <color rgb="FFEF0093"/>
-      <color rgb="FFDC0002"/>
-      <color rgb="FFDD270F"/>
-      <color rgb="FFD0B000"/>
-      <color rgb="FFFFCB00"/>
-      <color rgb="FF00C9D1"/>
+      <color rgb="FFD86295"/>
+      <color rgb="FFCE65D8"/>
+      <color rgb="FFA45CD8"/>
+      <color rgb="FFBA69F0"/>
+      <color rgb="FFB726FF"/>
+      <color rgb="FF3138DA"/>
+      <color rgb="FFDADA18"/>
+      <color rgb="FF30EA81"/>
+      <color rgb="FFEAE657"/>
+      <color rgb="FF77E3EA"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1744,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EAB0204-B451-8F42-930D-BA7D94248E53}">
   <dimension ref="A3:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A26" zoomScale="214" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1938,16 +3005,16 @@
       <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="52" t="s">
+      <c r="G20" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="42" t="s">
+      <c r="H20" s="43" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1961,39 +3028,39 @@
       <c r="C21" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="43" t="s">
+      <c r="G21" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="23">
         <v>477</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="12">
+      <c r="A22" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="13">
         <v>241</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="G22" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="24">
+      <c r="H22" s="25">
         <v>1881</v>
       </c>
     </row>
@@ -2007,39 +3074,39 @@
       <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H23" s="27">
         <v>146580</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="8">
+      <c r="A24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="9">
         <v>353</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="29">
         <v>7499</v>
       </c>
     </row>
@@ -2053,277 +3120,277 @@
       <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="47" t="s">
+      <c r="G25" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="31">
         <v>6432</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="8">
+      <c r="A26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="9">
         <v>372</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="G26" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="33">
         <v>137373</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="8">
+      <c r="A27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="9">
         <v>460</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="49" t="s">
+      <c r="G27" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="34">
+      <c r="H27" s="35">
         <v>8898</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="8">
+      <c r="A28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="9">
         <v>481</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="53" t="s">
+      <c r="G28" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="36">
+      <c r="H28" s="37">
         <v>225399</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="8">
+      <c r="A29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="9">
         <v>569</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="F29" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="G29" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="39">
         <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="8">
+      <c r="A30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="9">
         <v>652</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G30" s="51" t="s">
+      <c r="G30" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="40">
+      <c r="H30" s="41">
         <v>36000</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="16">
+      <c r="A31" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="17">
         <v>658</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="54" t="s">
+      <c r="F31" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="54" t="s">
+      <c r="G31" s="55" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="8">
+      <c r="A32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="9">
         <v>720</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="57" t="s">
+      <c r="D32" s="58" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="54">
+      <c r="A33" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="55">
         <v>724</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="59" t="s">
+      <c r="D33" s="60" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="16">
+      <c r="A34" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="17">
         <v>744</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="17" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="54">
+      <c r="A35" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="55">
         <v>757</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="59" t="s">
+      <c r="D35" s="60" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" s="16">
+      <c r="A36" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="17">
         <v>766</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="8">
+      <c r="A37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="9">
         <v>778</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="8">
+      <c r="A38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="9">
         <v>810</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="57" t="s">
+      <c r="D38" s="58" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="8">
+      <c r="A39" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="9">
         <v>850</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="59" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" s="8">
+      <c r="A40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="9">
         <v>898</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="59" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2342,86 +3409,86 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="16">
+      <c r="A42" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="17">
         <v>951</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="20" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" s="8">
+      <c r="A43" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="9">
         <v>1015</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" s="8">
+      <c r="A44" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="9">
         <v>1092</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="55" t="s">
+      <c r="D44" s="56" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="16">
+      <c r="A45" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="17">
         <v>1149</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="18" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" s="8">
+      <c r="A46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="9">
         <v>1164</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="8">
+      <c r="A47" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="9">
         <v>1200</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="56" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2435,7 +3502,7 @@
       <c r="C48" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2449,35 +3516,35 @@
       <c r="C49" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="16">
+      <c r="A50" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="17">
         <v>1275</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="8">
+      <c r="A51" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="9">
         <v>1296</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2491,21 +3558,21 @@
       <c r="C52" t="s">
         <v>23</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53" s="8">
+      <c r="A53" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="9">
         <v>1369</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2519,21 +3586,21 @@
       <c r="C54" t="s">
         <v>23</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55" s="8">
+      <c r="A55" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="9">
         <v>1498</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D55" s="56" t="s">
+      <c r="D55" s="57" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2566,30 +3633,30 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="8">
+      <c r="A58" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" s="9">
         <v>1675</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" s="16">
+      <c r="A59" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="17">
         <v>1730</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="21" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2603,21 +3670,21 @@
       <c r="C60" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="8">
+      <c r="A61" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="9">
         <v>1807</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2631,49 +3698,49 @@
       <c r="C62" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B63" s="12">
+      <c r="A63" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="13">
         <v>2612</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="12">
+      <c r="A64" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="13">
         <v>2616</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B65" s="8">
+      <c r="A65" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="9">
         <v>2751</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D65" s="12" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2685,12 +3752,446 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17CA361-77E0-B94C-8889-2F572D42E4DC}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="192" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" customWidth="1"/>
+    <col min="4" max="4" width="98" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="114" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="114">
+        <v>478</v>
+      </c>
+      <c r="C4" s="114"/>
+      <c r="D4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="64">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>556</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="67">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9">
+        <v>652</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="125" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="73">
+        <v>6006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>658</v>
+      </c>
+      <c r="C7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="80">
+        <v>147702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>744</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="124" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" s="85">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>950</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="92" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="88">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1077</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="91">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1164</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="94" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="95">
+        <v>84806</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="82">
+        <v>1275</v>
+      </c>
+      <c r="C12" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="96" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="97" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="98">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1296</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" s="99" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="100" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="101">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="75">
+        <v>1324</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="81" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="103" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="104">
+        <v>61707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="124" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="82">
+        <v>1640</v>
+      </c>
+      <c r="C15" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="126" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="105" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" s="107">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1675</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="108" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="109" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="110">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="75">
+        <v>1730</v>
+      </c>
+      <c r="C17" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="111" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="113">
+        <v>66039</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1807</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="115" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="117">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>2242</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="118" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="119" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="120">
+        <v>4257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>2611</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" s="121" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="122" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="123">
+        <v>50844</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="127" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="128" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="129">
+        <v>137447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>